<commit_message>
excel upd gazprom graf
</commit_message>
<xml_diff>
--- a/Course lll/Excel/sem_4/BaranovAV_Pi19-3_P4.xlsx
+++ b/Course lll/Excel/sem_4/BaranovAV_Pi19-3_P4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/FA19/Course lll/Excel/sem_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119FE13A-E20E-D84B-BB73-01DB85620C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7DC2B2-062D-5A46-9AF9-FEC874AA41E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="460" windowWidth="29020" windowHeight="17540" activeTab="2" xr2:uid="{2DE75494-FFD9-2547-9B90-3E4FE01A7980}"/>
+    <workbookView xWindow="260" yWindow="460" windowWidth="29020" windowHeight="17540" activeTab="1" xr2:uid="{2DE75494-FFD9-2547-9B90-3E4FE01A7980}"/>
   </bookViews>
   <sheets>
     <sheet name="Сбербанк" sheetId="2" r:id="rId1"/>
@@ -192,7 +192,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;₽&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;₽&quot;"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -409,163 +409,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="43">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;₽&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;₽&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;₽&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;₽&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;₽&quot;"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;₽&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="7" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -624,6 +478,189 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;₽&quot;"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;₽&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;₽&quot;"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;₽&quot;"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;₽&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;₽&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="7" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="3" formatCode="#,##0"/>
       <fill>
         <patternFill patternType="none">
@@ -646,43 +683,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -12523,286 +12523,286 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="94"/>
                 <c:pt idx="0">
-                  <c:v>1728709624.8708887</c:v>
+                  <c:v>742261177.94126344</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1743468089.8612018</c:v>
+                  <c:v>738458230.53840053</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1786460140.0503752</c:v>
+                  <c:v>727380079.40832162</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1816893744.8751204</c:v>
+                  <c:v>719537976.68937433</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1907919556.896121</c:v>
+                  <c:v>696082530.90649915</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1914794618.2270122</c:v>
+                  <c:v>694310971.55733943</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2045879120.9360058</c:v>
+                  <c:v>660533239.96669328</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1867035858.8484209</c:v>
+                  <c:v>706617403.83616924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1836877256.4769111</c:v>
+                  <c:v>714388644.18114996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1724584588.0723538</c:v>
+                  <c:v>743324113.55075932</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1667292410.3149266</c:v>
+                  <c:v>758087108.12709069</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1734209673.9356017</c:v>
+                  <c:v>740843930.46193576</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1774085029.6547709</c:v>
+                  <c:v>730568886.23680902</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1715326172.1467535</c:v>
+                  <c:v>745709813.47429442</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1769959992.8562362</c:v>
+                  <c:v>731631821.84630489</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1803876962.0886331</c:v>
+                  <c:v>722892129.05711675</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1865569179.0978308</c:v>
+                  <c:v>706995336.49732327</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1747043121.7532654</c:v>
+                  <c:v>737537019.67683744</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1680492528.0702379</c:v>
+                  <c:v>754685714.17670393</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1835960581.6327925</c:v>
+                  <c:v>714624852.09437132</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1836418919.054852</c:v>
+                  <c:v>714506748.13776064</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1781876765.8297811</c:v>
+                  <c:v>728561118.97442806</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1748876471.441503</c:v>
+                  <c:v>737064603.85039485</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1736409693.5614867</c:v>
+                  <c:v>740277031.47020459</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1851452386.4984007</c:v>
+                  <c:v>710632938.36093128</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1727609615.057946</c:v>
+                  <c:v>742544627.43712902</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1643917201.7898965</c:v>
+                  <c:v>764110409.9142338</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1772710017.3885927</c:v>
+                  <c:v>730923198.10664105</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1638875490.1472428</c:v>
+                  <c:v>765409553.43695092</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1771793342.5444739</c:v>
+                  <c:v>731159406.01986241</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1709001115.7223337</c:v>
+                  <c:v>747339648.07552147</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1739709723.0003147</c:v>
+                  <c:v>739426682.98260784</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1687550924.3699529</c:v>
+                  <c:v>752866913.24489999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1812585373.1077619</c:v>
+                  <c:v>720648153.88151455</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1801585274.9783361</c:v>
+                  <c:v>723482648.84017003</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1780960090.9856622</c:v>
+                  <c:v>728797326.8876493</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1798468580.508332</c:v>
+                  <c:v>724285755.74512243</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1793793538.8033259</c:v>
+                  <c:v>725490416.1025511</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1749793146.2856219</c:v>
+                  <c:v>736828395.9371736</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1691584293.6840758</c:v>
+                  <c:v>751827598.4267261</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1501649265.9826529</c:v>
+                  <c:v>800769878.04617977</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1712209477.6767495</c:v>
+                  <c:v>746512920.37924695</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1767118300.839468</c:v>
+                  <c:v>732364066.37729096</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1787376814.8944941</c:v>
+                  <c:v>727143871.49510026</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1808918673.7312868</c:v>
+                  <c:v>721592985.53439963</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1809377011.1533461</c:v>
+                  <c:v>721474881.57778907</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1773260022.295064</c:v>
+                  <c:v>730781473.35870826</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1681959207.820828</c:v>
+                  <c:v>754307781.5155499</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1629250404.2839949</c:v>
+                  <c:v>767889736.52577472</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1672792459.3796396</c:v>
+                  <c:v>756669860.64776289</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1817627084.7504156</c:v>
+                  <c:v>719349010.35879731</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1873544250.2416646</c:v>
+                  <c:v>704940327.65229797</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1792418526.5371478</c:v>
+                  <c:v>725844727.97238302</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1943394873.3635199</c:v>
+                  <c:v>686941284.66483474</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1959803353.0732472</c:v>
+                  <c:v>682713163.01817346</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1981711881.8476872</c:v>
+                  <c:v>677067793.89218438</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1964570062.262665</c:v>
+                  <c:v>681484881.86942267</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1925794716.3564382</c:v>
+                  <c:v>691476476.59868383</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1891877747.1240413</c:v>
+                  <c:v>700216169.38787198</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1834585569.3666141</c:v>
+                  <c:v>714979163.96420324</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1849710704.294575</c:v>
+                  <c:v>711081733.39605176</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1731826319.3408926</c:v>
+                  <c:v>741458071.03631115</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1733659669.0291305</c:v>
+                  <c:v>740985655.20986843</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1741268070.2353165</c:v>
+                  <c:v>739025129.5301317</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1708267775.8470385</c:v>
+                  <c:v>747528614.4060986</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1716792851.8973436</c:v>
+                  <c:v>745331880.81314039</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1753368178.1776853</c:v>
+                  <c:v>735907185.0756104</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1727884617.5111818</c:v>
+                  <c:v>742473765.06316257</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1671417447.1134615</c:v>
+                  <c:v>757024172.51759481</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1555366411.8480167</c:v>
+                  <c:v>786928094.3314116</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1620816995.7181017</c:v>
+                  <c:v>770062849.3274107</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1567466519.7903855</c:v>
+                  <c:v>783810149.87689042</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1638875490.1472428</c:v>
+                  <c:v>765409553.43695092</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1553441394.6753674</c:v>
+                  <c:v>787424130.94917631</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1588550041.2051184</c:v>
+                  <c:v>778377367.87280047</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1674534141.5834653</c:v>
+                  <c:v>756221065.61264241</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1543082968.9368246</c:v>
+                  <c:v>790093280.368577</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1074203786.1700399</c:v>
+                  <c:v>910913627.98127246</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>911677336.30777025</c:v>
+                  <c:v>952793290.99540925</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>874368670.15213346</c:v>
+                  <c:v>962406953.06351614</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>917910725.24777842</c:v>
+                  <c:v>951187077.18550432</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>975202903.00520563</c:v>
+                  <c:v>936424082.60917306</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>662616781.16068268</c:v>
+                  <c:v>1016970981.0176367</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>685166982.32600594</c:v>
+                  <c:v>1011160266.3523928</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>695617075.54896069</c:v>
+                  <c:v>1008467496.1416699</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>967869504.25225496</c:v>
+                  <c:v>938313745.91494346</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1188329804.2628348</c:v>
+                  <c:v>881505742.7852205</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1383031541.1536756</c:v>
+                  <c:v>831335182.01701617</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1304289172.0438676</c:v>
+                  <c:v>851625441.76272595</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1213080025.0540435</c:v>
+                  <c:v>875128129.12824535</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1264780486.2623458</c:v>
+                  <c:v>861806002.82256401</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1372214777.9930732</c:v>
+                  <c:v>834122435.39302754</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1386698240.5301511</c:v>
+                  <c:v>830390350.36413097</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1378081496.995434</c:v>
+                  <c:v>832610704.74841118</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15905,22 +15905,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B824C3C8-38FF-D64E-9AFE-CECBF41359A3}" name="ГАЗПРОМ_1" displayName="ГАЗПРОМ_1" ref="A1:G96" totalsRowCount="1" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25">
   <autoFilter ref="A1:G95" xr:uid="{B824C3C8-38FF-D64E-9AFE-CECBF41359A3}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{088CE3E2-D366-2944-B5D4-B2F9E29F9FB5}" name="Газпром-цена" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{06EE5DA9-1484-854F-A399-3739207D3BDC}" name="Газпром-объем" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{306E8154-9F9E-F240-B87C-6391BC878910}" name="h=k1*x+k0" totalsRowFunction="sum" dataDxfId="20">
-      <calculatedColumnFormula>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{088CE3E2-D366-2944-B5D4-B2F9E29F9FB5}" name="Газпром-цена" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{06EE5DA9-1484-854F-A399-3739207D3BDC}" name="Газпром-объем" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{306E8154-9F9E-F240-B87C-6391BC878910}" name="h=k1*x+k0" totalsRowFunction="sum" dataDxfId="0">
+      <calculatedColumnFormula>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F45DCDEA-8757-AD46-AFA5-0428B52D69E4}" name="y-h" totalsRowFunction="sum" dataDxfId="19">
+    <tableColumn id="4" xr3:uid="{F45DCDEA-8757-AD46-AFA5-0428B52D69E4}" name="y-h" totalsRowFunction="sum" dataDxfId="22">
       <calculatedColumnFormula>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{6BC82FD8-F740-384C-BB0F-7CAE1F556B3F}" name="(y-h)^2" totalsRowFunction="sum" dataDxfId="18">
+    <tableColumn id="5" xr3:uid="{6BC82FD8-F740-384C-BB0F-7CAE1F556B3F}" name="(y-h)^2" totalsRowFunction="sum" dataDxfId="21">
       <calculatedColumnFormula>ГАЗПРОМ_1[[#This Row],[y-h]]^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D4555C06-F51D-A84A-B204-C69E65E6106A}" name="x^2" totalsRowFunction="custom" dataDxfId="17">
+    <tableColumn id="6" xr3:uid="{D4555C06-F51D-A84A-B204-C69E65E6106A}" name="x^2" totalsRowFunction="custom" dataDxfId="20">
       <calculatedColumnFormula>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</calculatedColumnFormula>
       <totalsRowFormula>SUM(F2:F95)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0865C2AF-4F42-3644-8518-F733AAD6D07F}" name="x*y" totalsRowFunction="custom" dataDxfId="16">
+    <tableColumn id="7" xr3:uid="{0865C2AF-4F42-3644-8518-F733AAD6D07F}" name="x*y" totalsRowFunction="custom" dataDxfId="19">
       <calculatedColumnFormula>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]*ГАЗПРОМ_1[[#This Row],[Газпром-объем]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(G2:G95)</totalsRowFormula>
     </tableColumn>
@@ -15930,24 +15930,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{77AD8F1E-AC5C-5040-9EC7-5B05B1A70895}" name="ВТБ_1" displayName="ВТБ_1" ref="A1:G95" totalsRowCount="1" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{77AD8F1E-AC5C-5040-9EC7-5B05B1A70895}" name="ВТБ_1" displayName="ВТБ_1" ref="A1:G95" totalsRowCount="1" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="A1:G94" xr:uid="{77AD8F1E-AC5C-5040-9EC7-5B05B1A70895}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AEA07C9A-CAE9-2C4D-8DD7-9A96D583A1DE}" name="Втб ао цена" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{26B9649D-4C72-F343-B8A3-CC0C5C2736BA}" name="Втб ао объем" totalsRowFunction="sum" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{2382D00F-93F9-B548-8B65-401CA6E40CA2}" name="h=k1*x+k0" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="9">
+    <tableColumn id="1" xr3:uid="{AEA07C9A-CAE9-2C4D-8DD7-9A96D583A1DE}" name="Втб ао цена" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{26B9649D-4C72-F343-B8A3-CC0C5C2736BA}" name="Втб ао объем" totalsRowFunction="sum" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{2382D00F-93F9-B548-8B65-401CA6E40CA2}" name="h=k1*x+k0" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11">
       <calculatedColumnFormula>k1_v*ВТБ_1[[#This Row],[Втб ао цена]]+k0_v</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9F50CDE5-D894-3547-AAB2-5DA3D5F73E0F}" name="y-h" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="8">
+    <tableColumn id="4" xr3:uid="{9F50CDE5-D894-3547-AAB2-5DA3D5F73E0F}" name="y-h" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9">
       <calculatedColumnFormula>ВТБ_1[[#This Row],[Втб ао объем]]-ВТБ_1[[#This Row],[h=k1*x+k0]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{9E80DAF0-BF7A-0A45-A3D7-835E67AE9BE6}" name="(y-h)^2" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="7">
+    <tableColumn id="5" xr3:uid="{9E80DAF0-BF7A-0A45-A3D7-835E67AE9BE6}" name="(y-h)^2" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7">
       <calculatedColumnFormula>ВТБ_1[[#This Row],[y-h]]^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A1CF8366-FE70-EF4F-A230-576DE588F15C}" name="x^2" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="6">
+    <tableColumn id="6" xr3:uid="{A1CF8366-FE70-EF4F-A230-576DE588F15C}" name="x^2" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5">
       <calculatedColumnFormula>ВТБ_1[[#This Row],[Втб ао цена]]^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BF827D37-FB6B-474F-A710-F38541F935FA}" name="x*y" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="5">
+    <tableColumn id="7" xr3:uid="{BF827D37-FB6B-474F-A710-F38541F935FA}" name="x*y" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3">
       <calculatedColumnFormula>ВТБ_1[[#This Row],[Втб ао цена]]*ВТБ_1[[#This Row],[Втб ао объем]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -21064,8 +21064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C90DBE2-E229-054C-AD80-0349C463BCC4}">
   <dimension ref="A1:Q164"/>
   <sheetViews>
-    <sheetView zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21110,16 +21110,16 @@
         <v>638968460</v>
       </c>
       <c r="C2">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1728709624.8708887</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>742261177.94126344</v>
       </c>
       <c r="D2" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1089741164.8708887</v>
+        <v>-103292717.94126344</v>
       </c>
       <c r="E2" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.1875358064141614E+18</v>
+        <v>1.0669385579693406E+16</v>
       </c>
       <c r="F2">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21138,16 +21138,16 @@
         <v>495283520</v>
       </c>
       <c r="C3">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1743468089.8612018</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>738458230.53840053</v>
       </c>
       <c r="D3" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1248184569.8612018</v>
+        <v>-243174710.53840053</v>
       </c>
       <c r="E3" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.5579647204395932E+18</v>
+        <v>5.9133939845434888E+16</v>
       </c>
       <c r="F3">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21166,16 +21166,16 @@
         <v>733770920</v>
       </c>
       <c r="C4">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1786460140.0503752</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>727380079.40832162</v>
       </c>
       <c r="D4" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1052689220.0503752</v>
+        <v>6390840.591678381</v>
       </c>
       <c r="E4" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.1081545940102673E+18</v>
+        <v>40842843468244.078</v>
       </c>
       <c r="F4">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21194,16 +21194,16 @@
         <v>953973070</v>
       </c>
       <c r="C5">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1816893744.8751204</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>719537976.68937433</v>
       </c>
       <c r="D5" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-862920674.8751204</v>
+        <v>234435093.31062567</v>
       </c>
       <c r="E5" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>7.4463209112693325E+17</v>
+        <v>5.4959812975561768E+16</v>
       </c>
       <c r="F5">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21222,16 +21222,16 @@
         <v>986321760</v>
       </c>
       <c r="C6">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1907919556.896121</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>696082530.90649915</v>
       </c>
       <c r="D6" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-921597796.89612103</v>
+        <v>290239229.09350085</v>
       </c>
       <c r="E6" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>8.4934249924378394E+17</v>
+        <v>8.4238810104789664E+16</v>
       </c>
       <c r="F6">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21265,16 +21265,16 @@
         <v>813775000</v>
       </c>
       <c r="C7">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1914794618.2270122</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>694310971.55733943</v>
       </c>
       <c r="D7" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1101019618.2270122</v>
+        <v>119464028.44266057</v>
       </c>
       <c r="E7" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.2122441997207557E+18</v>
+        <v>1.4271654091748814E+16</v>
       </c>
       <c r="F7">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21293,16 +21293,16 @@
         <v>769293390</v>
       </c>
       <c r="C8">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>2045879120.9360058</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>660533239.96669328</v>
       </c>
       <c r="D8" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1276585730.9360058</v>
+        <v>108760150.03330672</v>
       </c>
       <c r="E8" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.6296711284294162E+18</v>
+        <v>1.1828770235267388E+16</v>
       </c>
       <c r="F8">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21321,16 +21321,16 @@
         <v>879462790</v>
       </c>
       <c r="C9">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1867035858.8484209</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>706617403.83616924</v>
       </c>
       <c r="D9" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-987573068.84842086</v>
+        <v>172845386.16383076</v>
       </c>
       <c r="E9" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>9.7530056631468774E+17</v>
+        <v>2.9875527518123776E+16</v>
       </c>
       <c r="F9">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21349,16 +21349,16 @@
         <v>635494510</v>
       </c>
       <c r="C10">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1836877256.4769111</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>714388644.18114996</v>
       </c>
       <c r="D10" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1201382746.4769111</v>
+        <v>-78894134.18114996</v>
       </c>
       <c r="E10" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.443320503532406E+18</v>
+        <v>6224284408193294</v>
       </c>
       <c r="F10">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21377,16 +21377,16 @@
         <v>1035314530</v>
       </c>
       <c r="C11">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1724584588.0723538</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>743324113.55075932</v>
       </c>
       <c r="D11" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-689270058.07235384</v>
+        <v>291990416.44924068</v>
       </c>
       <c r="E11" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>4.7509321295506605E+17</v>
+        <v>8.5258403298201008E+16</v>
       </c>
       <c r="F11">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21405,16 +21405,16 @@
         <v>1120379070</v>
       </c>
       <c r="C12">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1667292410.3149266</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>758087108.12709069</v>
       </c>
       <c r="D12" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-546913340.31492662</v>
+        <v>362291961.87290931</v>
       </c>
       <c r="E12" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>2.9911420181443072E+17</v>
+        <v>1.3125546563772157E+17</v>
       </c>
       <c r="F12">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21433,16 +21433,16 @@
         <v>1035969280</v>
       </c>
       <c r="C13">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1734209673.9356017</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>740843930.46193576</v>
       </c>
       <c r="D13" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-698240393.93560171</v>
+        <v>295125349.53806424</v>
       </c>
       <c r="E13" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>4.8753964772334426E+17</v>
+        <v>8.7098971939964592E+16</v>
       </c>
       <c r="F13">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21461,16 +21461,16 @@
         <v>1050788060</v>
       </c>
       <c r="C14">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1774085029.6547709</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>730568886.23680902</v>
       </c>
       <c r="D14" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-723296969.65477085</v>
+        <v>320219173.76319098</v>
       </c>
       <c r="E14" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>5.2315850631177453E+17</v>
+        <v>1.025403192455807E+17</v>
       </c>
       <c r="F14">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21489,16 +21489,16 @@
         <v>1056510690</v>
       </c>
       <c r="C15">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1715326172.1467535</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>745709813.47429442</v>
       </c>
       <c r="D15" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-658815482.14675355</v>
+        <v>310800876.52570558</v>
       </c>
       <c r="E15" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>4.3403783951625933E+17</v>
+        <v>9.659718484914688E+16</v>
       </c>
       <c r="F15">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21517,16 +21517,16 @@
         <v>1110186930</v>
       </c>
       <c r="C16">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1769959992.8562362</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>731631821.84630489</v>
       </c>
       <c r="D16" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-659773062.85623622</v>
+        <v>378555108.15369511</v>
       </c>
       <c r="E16" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>4.3530049447069901E+17</v>
+        <v>1.4330396990925579E+17</v>
       </c>
       <c r="F16">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21545,16 +21545,16 @@
         <v>2038314440</v>
       </c>
       <c r="C17">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1803876962.0886331</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>722892129.05711675</v>
       </c>
       <c r="D17" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>234437477.91136694</v>
+        <v>1315422310.9428833</v>
       </c>
       <c r="E17" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>5.4960931049442664E+16</v>
+        <v>1.7303358561263155E+18</v>
       </c>
       <c r="F17">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21573,16 +21573,16 @@
         <v>1377698400</v>
       </c>
       <c r="C18">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1865569179.0978308</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>706995336.49732327</v>
       </c>
       <c r="D18" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-487870779.09783077</v>
+        <v>670703063.50267673</v>
       </c>
       <c r="E18" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>2.3801789709752438E+17</v>
+        <v>4.4984259939187558E+17</v>
       </c>
       <c r="F18">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21601,16 +21601,16 @@
         <v>1168270410</v>
       </c>
       <c r="C19">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1747043121.7532654</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>737537019.67683744</v>
       </c>
       <c r="D19" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-578772711.75326538</v>
+        <v>430733390.32316256</v>
       </c>
       <c r="E19" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>3.3497785187022842E+17</v>
+        <v>1.8553125353928592E+17</v>
       </c>
       <c r="F19">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21629,16 +21629,16 @@
         <v>885913470</v>
       </c>
       <c r="C20">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1680492528.0702379</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>754685714.17670393</v>
       </c>
       <c r="D20" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-794579058.07023787</v>
+        <v>131227755.82329607</v>
       </c>
       <c r="E20" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>6.313558795237865E+17</v>
+        <v>1.7220723898418616E+16</v>
       </c>
       <c r="F20">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21657,16 +21657,16 @@
         <v>1004959980</v>
       </c>
       <c r="C21">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1835960581.6327925</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>714624852.09437132</v>
       </c>
       <c r="D21" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-831000601.63279247</v>
+        <v>290335127.90562868</v>
       </c>
       <c r="E21" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>6.905619999140631E+17</v>
+        <v>8.429448649597776E+16</v>
       </c>
       <c r="F21">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21685,16 +21685,16 @@
         <v>851294800</v>
       </c>
       <c r="C22">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1836418919.054852</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>714506748.13776064</v>
       </c>
       <c r="D22" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-985124119.05485201</v>
+        <v>136788051.86223936</v>
       </c>
       <c r="E22" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>9.7046952994359821E+17</v>
+        <v>1.8710971132266684E+16</v>
       </c>
       <c r="F22">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21713,16 +21713,16 @@
         <v>797896850</v>
       </c>
       <c r="C23">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1781876765.8297811</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>728561118.97442806</v>
       </c>
       <c r="D23" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-983979915.82978106</v>
+        <v>69335731.025571942</v>
       </c>
       <c r="E23" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>9.6821647475638298E+17</v>
+        <v>4807443596850460</v>
       </c>
       <c r="F23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21741,16 +21741,16 @@
         <v>857933800</v>
       </c>
       <c r="C24">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1748876471.441503</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>737064603.85039485</v>
       </c>
       <c r="D24" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-890942671.44150305</v>
+        <v>120869196.14960515</v>
       </c>
       <c r="E24" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>7.9377884379532211E+17</v>
+        <v>1.4609362577851726E+16</v>
       </c>
       <c r="F24">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21769,16 +21769,16 @@
         <v>691989260</v>
       </c>
       <c r="C25">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1736409693.5614867</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>740277031.47020459</v>
       </c>
       <c r="D25" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1044420433.5614867</v>
+        <v>-48287771.470204592</v>
       </c>
       <c r="E25" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.0908140420407639E+18</v>
+        <v>2331708873558704.5</v>
       </c>
       <c r="F25">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21797,16 +21797,16 @@
         <v>983856510</v>
       </c>
       <c r="C26">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1851452386.4984007</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>710632938.36093128</v>
       </c>
       <c r="D26" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-867595876.49840069</v>
+        <v>273223571.63906872</v>
       </c>
       <c r="E26" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>7.527226049170281E+17</v>
+        <v>7.4651120099209312E+16</v>
       </c>
       <c r="F26">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21825,16 +21825,16 @@
         <v>652102830</v>
       </c>
       <c r="C27">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1727609615.057946</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>742544627.43712902</v>
       </c>
       <c r="D27" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1075506785.057946</v>
+        <v>-90441797.437129021</v>
       </c>
       <c r="E27" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.1567148447056788E+18</v>
+        <v>8179718723658677</v>
       </c>
       <c r="F27">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21853,16 +21853,16 @@
         <v>919520350</v>
       </c>
       <c r="C28">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1643917201.7898965</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>764110409.9142338</v>
       </c>
       <c r="D28" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-724396851.78989649</v>
+        <v>155409940.0857662</v>
       </c>
       <c r="E28" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>5.2475079888311328E+17</v>
+        <v>2.415224947746144E+16</v>
       </c>
       <c r="F28">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21881,16 +21881,16 @@
         <v>718069290</v>
       </c>
       <c r="C29">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1772710017.3885927</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>730923198.10664105</v>
       </c>
       <c r="D29" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1054640727.3885927</v>
+        <v>-12853908.106641054</v>
       </c>
       <c r="E29" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.11226706386674E+18</v>
+        <v>165222953613972.62</v>
       </c>
       <c r="F29">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21909,16 +21909,16 @@
         <v>821523460</v>
       </c>
       <c r="C30">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1638875490.1472428</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>765409553.43695092</v>
       </c>
       <c r="D30" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-817352030.14724278</v>
+        <v>56113906.563049078</v>
       </c>
       <c r="E30" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>6.6806434118581926E+17</v>
+        <v>3148770509766602.5</v>
       </c>
       <c r="F30">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21937,16 +21937,16 @@
         <v>472091480</v>
       </c>
       <c r="C31">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1771793342.5444739</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>731159406.01986241</v>
       </c>
       <c r="D31" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1299701862.5444739</v>
+        <v>-259067926.01986241</v>
       </c>
       <c r="E31" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.6892249315015744E+18</v>
+        <v>6.7116190292232904E+16</v>
       </c>
       <c r="F31">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21965,16 +21965,16 @@
         <v>533051950</v>
       </c>
       <c r="C32">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1709001115.7223337</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>747339648.07552147</v>
       </c>
       <c r="D32" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1175949165.7223337</v>
+        <v>-214287698.07552147</v>
       </c>
       <c r="E32" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.3828564403630525E+18</v>
+        <v>4.5919217546505848E+16</v>
       </c>
       <c r="F32">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -21993,16 +21993,16 @@
         <v>543868920</v>
       </c>
       <c r="C33">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1739709723.0003147</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>739426682.98260784</v>
       </c>
       <c r="D33" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1195840803.0003147</v>
+        <v>-195557762.98260784</v>
       </c>
       <c r="E33" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.4300352261204375E+18</v>
+        <v>3.8242838662761824E+16</v>
       </c>
       <c r="F33">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22021,16 +22021,16 @@
         <v>654231910</v>
       </c>
       <c r="C34">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1687550924.3699529</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>752866913.24489999</v>
       </c>
       <c r="D34" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1033319014.3699529</v>
+        <v>-98635003.244899988</v>
       </c>
       <c r="E34" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.067748185458491E+18</v>
+        <v>9728863865121432</v>
       </c>
       <c r="F34">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22049,16 +22049,16 @@
         <v>646257900</v>
       </c>
       <c r="C35">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1812585373.1077619</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>720648153.88151455</v>
       </c>
       <c r="D35" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1166327473.1077619</v>
+        <v>-74390253.881514549</v>
       </c>
       <c r="E35" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.3603197745259369E+18</v>
+        <v>5533909872556190</v>
       </c>
       <c r="F35">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22077,16 +22077,16 @@
         <v>727388150</v>
       </c>
       <c r="C36">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1801585274.9783361</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>723482648.84017003</v>
       </c>
       <c r="D36" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1074197124.9783361</v>
+        <v>3905501.1598299742</v>
       </c>
       <c r="E36" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.153899463311723E+18</v>
+        <v>15252939309433.273</v>
       </c>
       <c r="F36">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22114,16 +22114,16 @@
         <v>785173850</v>
       </c>
       <c r="C37">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1780960090.9856622</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>728797326.8876493</v>
       </c>
       <c r="D37" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-995786240.98566222</v>
+        <v>56376523.112350702</v>
       </c>
       <c r="E37" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>9.9159023773635533E+17</v>
+        <v>3178312358237413</v>
       </c>
       <c r="F37">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22154,16 +22154,16 @@
         <v>632658380</v>
       </c>
       <c r="C38">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1798468580.508332</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>724285755.74512243</v>
       </c>
       <c r="D38" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1165810200.508332</v>
+        <v>-91627375.745122433</v>
       </c>
       <c r="E38" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.3591134236092772E+18</v>
+        <v>8395575985937851</v>
       </c>
       <c r="F38">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22194,16 +22194,16 @@
         <v>614480400</v>
       </c>
       <c r="C39">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1793793538.8033259</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>725490416.1025511</v>
       </c>
       <c r="D39" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1179313138.8033259</v>
+        <v>-111010016.1025511</v>
       </c>
       <c r="E39" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.3907794793541527E+18</v>
+        <v>1.2323223675088656E+16</v>
       </c>
       <c r="F39">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22222,16 +22222,16 @@
         <v>642613120</v>
       </c>
       <c r="C40">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1749793146.2856219</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>736828395.9371736</v>
       </c>
       <c r="D40" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1107180026.2856219</v>
+        <v>-94215275.937173605</v>
       </c>
       <c r="E40" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.2258476106058304E+18</v>
+        <v>8876518219917764</v>
       </c>
       <c r="F40">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22254,16 +22254,16 @@
         <v>731620780</v>
       </c>
       <c r="C41">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1691584293.6840758</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>751827598.4267261</v>
       </c>
       <c r="D41" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-959963513.68407583</v>
+        <v>-20206818.426726103</v>
       </c>
       <c r="E41" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>9.2152994760467686E+17</v>
+        <v>408315510930677.56</v>
       </c>
       <c r="F41">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22287,16 +22287,16 @@
         <v>941606540</v>
       </c>
       <c r="C42">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1501649265.9826529</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>800769878.04617977</v>
       </c>
       <c r="D42" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-560042725.9826529</v>
+        <v>140836661.95382023</v>
       </c>
       <c r="E42" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>3.1364785492608083E+17</v>
+        <v>1.9834965350294636E+16</v>
       </c>
       <c r="F42">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22315,16 +22315,16 @@
         <v>662677050</v>
       </c>
       <c r="C43">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1712209477.6767495</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>746512920.37924695</v>
       </c>
       <c r="D43" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1049532427.6767495</v>
+        <v>-83835870.37924695</v>
       </c>
       <c r="E43" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.1015183167450514E+18</v>
+        <v>7028453162245896</v>
       </c>
       <c r="F43">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22343,16 +22343,16 @@
         <v>538549300</v>
       </c>
       <c r="C44">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1767118300.839468</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>732364066.37729096</v>
       </c>
       <c r="D44" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1228569000.839468</v>
+        <v>-193814766.37729096</v>
       </c>
       <c r="E44" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.5093817898236887E+18</v>
+        <v>3.7564163665883872E+16</v>
       </c>
       <c r="F44">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22371,16 +22371,16 @@
         <v>505531930</v>
       </c>
       <c r="C45">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1787376814.8944941</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>727143871.49510026</v>
       </c>
       <c r="D45" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1281844884.8944941</v>
+        <v>-221611941.49510026</v>
       </c>
       <c r="E45" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.6431263089301788E+18</v>
+        <v>4.9111852613227744E+16</v>
       </c>
       <c r="F45">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22399,16 +22399,16 @@
         <v>472860350</v>
       </c>
       <c r="C46">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1808918673.7312868</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>721592985.53439963</v>
       </c>
       <c r="D46" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1336058323.7312868</v>
+        <v>-248732635.53439963</v>
       </c>
       <c r="E46" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.7850518444116559E+18</v>
+        <v>6.186792397988848E+16</v>
       </c>
       <c r="F46">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22427,16 +22427,16 @@
         <v>567536440</v>
       </c>
       <c r="C47">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1809377011.1533461</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>721474881.57778907</v>
       </c>
       <c r="D47" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1241840571.1533461</v>
+        <v>-153938441.57778907</v>
       </c>
       <c r="E47" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.5421680041624689E+18</v>
+        <v>2.369704379539838E+16</v>
       </c>
       <c r="F47">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22458,16 +22458,16 @@
         <v>409341480</v>
       </c>
       <c r="C48">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1773260022.295064</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>730781473.35870826</v>
       </c>
       <c r="D48" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1363918542.295064</v>
+        <v>-321439993.35870826</v>
       </c>
       <c r="E48" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.8602737900162921E+18</v>
+        <v>1.0332366933044642E+17</v>
       </c>
       <c r="F48">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22486,16 +22486,16 @@
         <v>735320710</v>
       </c>
       <c r="C49">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1681959207.820828</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>754307781.5155499</v>
       </c>
       <c r="D49" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-946638497.82082796</v>
+        <v>-18987071.515549898</v>
       </c>
       <c r="E49" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>8.9612444555647373E+17</v>
+        <v>360508884736606.31</v>
       </c>
       <c r="F49">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22518,16 +22518,16 @@
         <v>680484920</v>
       </c>
       <c r="C50">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1629250404.2839949</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>767889736.52577472</v>
       </c>
       <c r="D50" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-948765484.28399491</v>
+        <v>-87404816.525774717</v>
       </c>
       <c r="E50" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>9.0015594416864346E+17</v>
+        <v>7639601951904341</v>
       </c>
       <c r="F50">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22552,16 +22552,16 @@
         <v>508472070</v>
       </c>
       <c r="C51">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1672792459.3796396</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>756669860.64776289</v>
       </c>
       <c r="D51" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1164320389.3796396</v>
+        <v>-248197790.64776289</v>
       </c>
       <c r="E51" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.3556419691251556E+18</v>
+        <v>6.1602143282430736E+16</v>
       </c>
       <c r="F51">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22586,16 +22586,16 @@
         <v>618092220</v>
       </c>
       <c r="C52">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1817627084.7504156</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>719349010.35879731</v>
       </c>
       <c r="D52" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1199534864.7504156</v>
+        <v>-101256790.35879731</v>
       </c>
       <c r="E52" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.4388838917517978E+18</v>
+        <v>1.0252937593765428E+16</v>
       </c>
       <c r="F52">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22620,16 +22620,16 @@
         <v>754410290</v>
       </c>
       <c r="C53">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1873544250.2416646</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>704940327.65229797</v>
       </c>
       <c r="D53" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1119133960.2416646</v>
+        <v>49469962.347702026</v>
       </c>
       <c r="E53" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.2524608209661919E+18</v>
+        <v>2447277174683056</v>
       </c>
       <c r="F53">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22654,16 +22654,16 @@
         <v>750182400</v>
       </c>
       <c r="C54">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1792418526.5371478</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>725844727.97238302</v>
       </c>
       <c r="D54" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1042236126.5371478</v>
+        <v>24337672.027616978</v>
       </c>
       <c r="E54" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.0862561434591575E+18</v>
+        <v>592322279723849.88</v>
       </c>
       <c r="F54">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22688,16 +22688,16 @@
         <v>683155600</v>
       </c>
       <c r="C55">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1943394873.3635199</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>686941284.66483474</v>
       </c>
       <c r="D55" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1260239273.3635199</v>
+        <v>-3785684.6648347378</v>
       </c>
       <c r="E55" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.5882030261278126E+18</v>
+        <v>14331408381564.9</v>
       </c>
       <c r="F55">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22716,16 +22716,16 @@
         <v>682977210</v>
       </c>
       <c r="C56">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1959803353.0732472</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>682713163.01817346</v>
       </c>
       <c r="D56" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1276826143.0732472</v>
+        <v>264046.98182654381</v>
       </c>
       <c r="E56" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.6302849996353042E+18</v>
+        <v>69720808611.707153</v>
       </c>
       <c r="F56">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22747,16 +22747,16 @@
         <v>572372360</v>
       </c>
       <c r="C57">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1981711881.8476872</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>677067793.89218438</v>
       </c>
       <c r="D57" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1409339521.8476872</v>
+        <v>-104695433.89218438</v>
       </c>
       <c r="E57" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.9862378878418678E+18</v>
+        <v>1.096113387787275E+16</v>
       </c>
       <c r="F57">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22791,16 +22791,16 @@
         <v>490084870</v>
       </c>
       <c r="C58">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1964570062.262665</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>681484881.86942267</v>
       </c>
       <c r="D58" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1474485192.262665</v>
+        <v>-191400011.86942267</v>
       </c>
       <c r="E58" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>2.1741065822018683E+18</v>
+        <v>3.6633964543615144E+16</v>
       </c>
       <c r="F58">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22837,16 +22837,16 @@
         <v>615131840</v>
       </c>
       <c r="C59">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1925794716.3564382</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>691476476.59868383</v>
       </c>
       <c r="D59" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1310662876.3564382</v>
+        <v>-76344636.598683834</v>
       </c>
       <c r="E59" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.717837175458932E+18</v>
+        <v>5828503537385095</v>
       </c>
       <c r="F59">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22879,16 +22879,16 @@
         <v>511657140</v>
       </c>
       <c r="C60">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1891877747.1240413</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>700216169.38787198</v>
       </c>
       <c r="D60" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1380220607.1240413</v>
+        <v>-188559029.38787198</v>
       </c>
       <c r="E60" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.9050089243298573E+18</v>
+        <v>3.5554507563696368E+16</v>
       </c>
       <c r="F60">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22919,16 +22919,16 @@
         <v>670673200</v>
       </c>
       <c r="C61">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1834585569.3666141</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>714979163.96420324</v>
       </c>
       <c r="D61" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1163912369.3666141</v>
+        <v>-44305963.964203238</v>
       </c>
       <c r="E61" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.3546920035646054E+18</v>
+        <v>1963018442797276</v>
       </c>
       <c r="F61">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -22947,16 +22947,16 @@
         <v>417311690</v>
       </c>
       <c r="C62">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1849710704.294575</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>711081733.39605176</v>
       </c>
       <c r="D62" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1432399014.294575</v>
+        <v>-293770043.39605176</v>
       </c>
       <c r="E62" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>2.0517669361520699E+18</v>
+        <v>8.6300838396918144E+16</v>
       </c>
       <c r="F62">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23000,16 +23000,16 @@
         <v>758630450</v>
       </c>
       <c r="C63">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1731826319.3408926</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>741458071.03631115</v>
       </c>
       <c r="D63" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-973195869.34089255</v>
+        <v>17172378.96368885</v>
       </c>
       <c r="E63" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>9.4711020010217562E+17</v>
+        <v>294890599272543.38</v>
       </c>
       <c r="F63">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23055,16 +23055,16 @@
         <v>675058310</v>
       </c>
       <c r="C64">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1733659669.0291305</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>740985655.20986843</v>
       </c>
       <c r="D64" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1058601359.0291305</v>
+        <v>-65927345.209868431</v>
       </c>
       <c r="E64" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.1206368373383219E+18</v>
+        <v>4346414846421162</v>
       </c>
       <c r="F64">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23110,16 +23110,16 @@
         <v>550336390</v>
       </c>
       <c r="C65">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1741268070.2353165</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>739025129.5301317</v>
       </c>
       <c r="D65" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1190931680.2353165</v>
+        <v>-188688739.5301317</v>
       </c>
       <c r="E65" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.4183182669881142E+18</v>
+        <v>3.5603440425469884E+16</v>
       </c>
       <c r="F65">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23138,16 +23138,16 @@
         <v>654967610</v>
       </c>
       <c r="C66">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1708267775.8470385</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>747528614.4060986</v>
       </c>
       <c r="D66" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1053300165.8470385</v>
+        <v>-92561004.406098604</v>
       </c>
       <c r="E66" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.1094412393733988E+18</v>
+        <v>8567539536665805</v>
       </c>
       <c r="F66">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23166,16 +23166,16 @@
         <v>457602320</v>
       </c>
       <c r="C67">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1716792851.8973436</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>745331880.81314039</v>
       </c>
       <c r="D67" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1259190531.8973436</v>
+        <v>-287729560.81314039</v>
       </c>
       <c r="E67" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.5855607956199153E+18</v>
+        <v>8.2788300165722656E+16</v>
       </c>
       <c r="F67">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23194,16 +23194,16 @@
         <v>439786830</v>
       </c>
       <c r="C68">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1753368178.1776853</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>735907185.0756104</v>
       </c>
       <c r="D68" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1313581348.1776853</v>
+        <v>-296120355.0756104</v>
       </c>
       <c r="E68" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.7254959582803052E+18</v>
+        <v>8.7687264690105584E+16</v>
       </c>
       <c r="F68">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23228,16 +23228,16 @@
         <v>403411200</v>
       </c>
       <c r="C69">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1727884617.5111818</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>742473765.06316257</v>
       </c>
       <c r="D69" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1324473417.5111818</v>
+        <v>-339062565.06316257</v>
       </c>
       <c r="E69" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.7542298336937495E+18</v>
+        <v>1.1496342302721134E+17</v>
       </c>
       <c r="F69">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23256,16 +23256,16 @@
         <v>441314630</v>
       </c>
       <c r="C70">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1671417447.1134615</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>757024172.51759481</v>
       </c>
       <c r="D70" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1230102817.1134615</v>
+        <v>-315709542.51759481</v>
       </c>
       <c r="E70" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.513152940670474E+18</v>
+        <v>9.9672515236669008E+16</v>
       </c>
       <c r="F70">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23302,16 +23302,16 @@
         <v>553952660</v>
       </c>
       <c r="C71">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1555366411.8480167</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>786928094.3314116</v>
       </c>
       <c r="D71" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1001413751.8480167</v>
+        <v>-232975434.3314116</v>
       </c>
       <c r="E71" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.0028295023903213E+18</v>
+        <v>5.427755300190988E+16</v>
       </c>
       <c r="F71">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23348,16 +23348,16 @@
         <v>708218240</v>
       </c>
       <c r="C72">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1620816995.7181017</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>770062849.3274107</v>
       </c>
       <c r="D72" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-912598755.71810174</v>
+        <v>-61844609.327410698</v>
       </c>
       <c r="E72" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>8.3283648893822758E+17</v>
+        <v>3824755702860054.5</v>
       </c>
       <c r="F72">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23394,16 +23394,16 @@
         <v>554088010</v>
       </c>
       <c r="C73">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1567466519.7903855</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>783810149.87689042</v>
       </c>
       <c r="D73" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1013378509.7903855</v>
+        <v>-229722139.87689042</v>
       </c>
       <c r="E73" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.0269360041049824E+18</v>
+        <v>5.2772261549617608E+16</v>
       </c>
       <c r="F73">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23440,16 +23440,16 @@
         <v>435896450</v>
       </c>
       <c r="C74">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1638875490.1472428</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>765409553.43695092</v>
       </c>
       <c r="D74" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1202979040.1472428</v>
+        <v>-329513103.43695092</v>
       </c>
       <c r="E74" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.4471585710335816E+18</v>
+        <v>1.0857888533665072E+17</v>
       </c>
       <c r="F74">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23486,16 +23486,16 @@
         <v>394617870</v>
       </c>
       <c r="C75">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1553441394.6753674</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>787424130.94917631</v>
       </c>
       <c r="D75" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1158823524.6753674</v>
+        <v>-392806260.94917631</v>
       </c>
       <c r="E75" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.3428719613410417E+18</v>
+        <v>1.5429675864087238E+17</v>
       </c>
       <c r="F75">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23532,16 +23532,16 @@
         <v>394761860</v>
       </c>
       <c r="C76">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1588550041.2051184</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>778377367.87280047</v>
       </c>
       <c r="D76" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1193788181.2051184</v>
+        <v>-383615507.87280047</v>
       </c>
       <c r="E76" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.4251302215850248E+18</v>
+        <v>1.4716085788050662E+17</v>
       </c>
       <c r="F76">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23578,16 +23578,16 @@
         <v>424906810</v>
       </c>
       <c r="C77">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1674534141.5834653</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>756221065.61264241</v>
       </c>
       <c r="D77" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1249627331.5834653</v>
+        <v>-331314255.61264241</v>
       </c>
       <c r="E77" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.5615684678404119E+18</v>
+        <v>1.0976913597215934E+17</v>
       </c>
       <c r="F77">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23624,16 +23624,16 @@
         <v>576420680</v>
       </c>
       <c r="C78">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1543082968.9368246</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>790093280.368577</v>
       </c>
       <c r="D78" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-966662288.93682456</v>
+        <v>-213672600.368577</v>
       </c>
       <c r="E78" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>9.3443598085258086E+17</v>
+        <v>4.5655980148269616E+16</v>
       </c>
       <c r="F78">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23670,16 +23670,16 @@
         <v>1077221090</v>
       </c>
       <c r="C79">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1074203786.1700399</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>910913627.98127246</v>
       </c>
       <c r="D79" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>3017303.8299601078</v>
+        <v>166307462.01872754</v>
       </c>
       <c r="E79" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>9104122402291.9355</v>
+        <v>2.7658171923110504E+16</v>
       </c>
       <c r="F79">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23716,16 +23716,16 @@
         <v>918359340</v>
       </c>
       <c r="C80">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>911677336.30777025</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>952793290.99540925</v>
       </c>
       <c r="D80" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>6682003.6922297478</v>
+        <v>-34433950.99540925</v>
       </c>
       <c r="E80" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>44649173342971.984</v>
+        <v>1185696981154245.8</v>
       </c>
       <c r="F80">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23762,16 +23762,16 @@
         <v>1185460410</v>
       </c>
       <c r="C81">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>874368670.15213346</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>962406953.06351614</v>
       </c>
       <c r="D81" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>311091739.84786654</v>
+        <v>223053456.93648386</v>
       </c>
       <c r="E81" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>9.6778070601572672E+16</v>
+        <v>4.9752844651315856E+16</v>
       </c>
       <c r="F81">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23808,16 +23808,16 @@
         <v>715634720</v>
       </c>
       <c r="C82">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>917910725.24777842</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>951187077.18550432</v>
       </c>
       <c r="D82" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-202276005.24777842</v>
+        <v>-235552357.18550432</v>
       </c>
       <c r="E82" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>4.091558229899928E+16</v>
+        <v>5.5484912975647408E+16</v>
       </c>
       <c r="F82">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23854,16 +23854,16 @@
         <v>514923280</v>
       </c>
       <c r="C83">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>975202903.00520563</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>936424082.60917306</v>
       </c>
       <c r="D83" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-460279623.00520563</v>
+        <v>-421500802.60917306</v>
       </c>
       <c r="E83" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>2.1185733135381421E+17</v>
+        <v>1.7766292660017706E+17</v>
       </c>
       <c r="F83">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23900,16 +23900,16 @@
         <v>763625060</v>
       </c>
       <c r="C84">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>662616781.16068268</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>1016970981.0176367</v>
       </c>
       <c r="D84" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>101008278.83931732</v>
+        <v>-253345921.01763666</v>
       </c>
       <c r="E84" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.020267239408128E+16</v>
+        <v>6.4184155696274592E+16</v>
       </c>
       <c r="F84">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23946,16 +23946,16 @@
         <v>1496648200</v>
       </c>
       <c r="C85">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>685166982.32600594</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>1011160266.3523928</v>
       </c>
       <c r="D85" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>811481217.67399406</v>
+        <v>485487933.64760721</v>
       </c>
       <c r="E85" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>6.585017666376681E+17</v>
+        <v>2.3569853371742346E+17</v>
       </c>
       <c r="F85">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -23992,16 +23992,16 @@
         <v>850735710</v>
       </c>
       <c r="C86">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>695617075.54896069</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>1008467496.1416699</v>
       </c>
       <c r="D86" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>155118634.45103931</v>
+        <v>-157731786.14166987</v>
       </c>
       <c r="E86" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>2.406179075395516E+16</v>
+        <v>2.487931635944148E+16</v>
       </c>
       <c r="F86">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -24038,16 +24038,16 @@
         <v>943229040</v>
       </c>
       <c r="C87">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>967869504.25225496</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>938313745.91494346</v>
       </c>
       <c r="D87" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-24640464.252254963</v>
+        <v>4915294.0850565434</v>
       </c>
       <c r="E87" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>607152478566654.75</v>
+        <v>24160115942591.84</v>
       </c>
       <c r="F87">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -24084,16 +24084,16 @@
         <v>1068549530</v>
       </c>
       <c r="C88">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1188329804.2628348</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>881505742.7852205</v>
       </c>
       <c r="D88" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-119780274.26283479</v>
+        <v>187043787.2147795</v>
       </c>
       <c r="E88" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.4347314102479922E+16</v>
+        <v>3.4985378335647708E+16</v>
       </c>
       <c r="F88">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -24130,16 +24130,16 @@
         <v>2274256090</v>
       </c>
       <c r="C89">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1383031541.1536756</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>831335182.01701617</v>
       </c>
       <c r="D89" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>891224548.84632444</v>
+        <v>1442920907.9829838</v>
       </c>
       <c r="E89" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>7.9428119646633459E+17</v>
+        <v>2.0820207466944384E+18</v>
       </c>
       <c r="F89">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -24176,16 +24176,16 @@
         <v>1151699700</v>
       </c>
       <c r="C90">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1304289172.0438676</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>851625441.76272595</v>
       </c>
       <c r="D90" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-152589472.04386759</v>
+        <v>300074258.23727405</v>
       </c>
       <c r="E90" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>2.3283546978626248E+16</v>
+        <v>9.004456045665024E+16</v>
       </c>
       <c r="F90">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -24222,16 +24222,16 @@
         <v>1119152560</v>
       </c>
       <c r="C91">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1213080025.0540435</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>875128129.12824535</v>
       </c>
       <c r="D91" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-93927465.054043531</v>
+        <v>244024430.87175465</v>
       </c>
       <c r="E91" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>8822368691478569</v>
+        <v>5.954792286228376E+16</v>
       </c>
       <c r="F91">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -24268,16 +24268,16 @@
         <v>949645980</v>
       </c>
       <c r="C92">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1264780486.2623458</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>861806002.82256401</v>
       </c>
       <c r="D92" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-315134506.26234579</v>
+        <v>87839977.177435994</v>
       </c>
       <c r="E92" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>9.9309757037212464E+16</v>
+        <v>7715861590532476</v>
       </c>
       <c r="F92">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -24314,16 +24314,16 @@
         <v>841671960</v>
       </c>
       <c r="C93">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1372214777.9930732</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>834122435.39302754</v>
       </c>
       <c r="D93" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-530542817.99307323</v>
+        <v>7549524.606972456</v>
       </c>
       <c r="E93" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>2.8147568172403123E+17</v>
+        <v>56995321791282.617</v>
       </c>
       <c r="F93">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -24360,16 +24360,16 @@
         <v>763622270</v>
       </c>
       <c r="C94">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1386698240.5301511</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>830390350.36413097</v>
       </c>
       <c r="D94" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-623075970.53015113</v>
+        <v>-66768080.364130974</v>
       </c>
       <c r="E94" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>3.8822366505208973E+17</v>
+        <v>4457976555511052</v>
       </c>
       <c r="F94">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -24406,16 +24406,16 @@
         <v>98371280</v>
       </c>
       <c r="C95">
-        <f>k1_*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0</f>
-        <v>1378081496.995434</v>
+        <f>k1_g*ГАЗПРОМ_1[[#This Row],[Газпром-цена]]+k0_g</f>
+        <v>832610704.74841118</v>
       </c>
       <c r="D95" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-объем]]-ГАЗПРОМ_1[[#This Row],[h=k1*x+k0]]</f>
-        <v>-1279710216.995434</v>
+        <v>-734239424.74841118</v>
       </c>
       <c r="E95" s="23">
         <f>ГАЗПРОМ_1[[#This Row],[y-h]]^2</f>
-        <v>1.6376582394825009E+18</v>
+        <v>5.3910753285487776E+17</v>
       </c>
       <c r="F95">
         <f>ГАЗПРОМ_1[[#This Row],[Газпром-цена]]^2</f>
@@ -24455,15 +24455,15 @@
       </c>
       <c r="C96">
         <f>SUBTOTAL(109,ГАЗПРОМ_1[h=k1*x+k0])</f>
-        <v>153802118824.22382</v>
+        <v>72013478820.000549</v>
       </c>
       <c r="D96">
         <f>SUBTOTAL(109,ГАЗПРОМ_1[y-h])</f>
-        <v>-81788640004.22374</v>
+        <v>-5.7554244995117188E-4</v>
       </c>
       <c r="E96">
         <f>SUBTOTAL(109,ГАЗПРОМ_1[(y-h)^2])</f>
-        <v>9.345394965462152E+19</v>
+        <v>8.8623239498155694E+18</v>
       </c>
       <c r="F96">
         <f>SUM(F2:F95)</f>
@@ -25868,8 +25868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69676C2E-1E8A-2C4F-9E2B-271EC833F27B}">
   <dimension ref="A1:S170"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+    <sheetView topLeftCell="A2" zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27052,7 +27052,7 @@
         <v>20873595494.000004</v>
       </c>
       <c r="I40">
-        <f t="array" ref="I40">MMULT(MINVERSE(I37:J38),K37:K38)</f>
+        <f>MMULT(MINVERSE(I37:J38),K37:K38)</f>
         <v>-10559914031872.281</v>
       </c>
     </row>

</xml_diff>